<commit_message>
Added Hardwarerelated architecture and images.
</commit_message>
<xml_diff>
--- a/DOCs/BOM.xlsx
+++ b/DOCs/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
   <si>
     <t xml:space="preserve">TRON Programming Contest 2025</t>
   </si>
@@ -336,7 +336,40 @@
     <t xml:space="preserve">The AD623 is specifically designed to amplify small differential signals while rejecting common-mode noise. It offers high input impedance and a high CMRR, both of which are essential for bio-signal measurement.</t>
   </si>
   <si>
-    <t xml:space="preserve">GROSS : Rs. 8314.38</t>
+    <t xml:space="preserve">Low Dropout Voltage Regulator (LDO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMS1117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step down voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power profile enhancement and user safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zener Diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1N4728A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protects against ESD Discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminates sudden ESD spikes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROSS : Rs. 8540.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***(The gross total also includes delivery charges, which are directly included in the “Total Cost” column)</t>
   </si>
 </sst>
 </file>
@@ -347,7 +380,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +457,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="14"/>
@@ -433,11 +474,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
       <u val="single"/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Latin Modern Math"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -488,11 +530,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -553,24 +595,28 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -823,10 +869,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="F1:R26"/>
+  <dimension ref="F1:R27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N27" activeCellId="0" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -836,7 +882,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="24.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="24.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="38.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="85.17"/>
   </cols>
@@ -1338,8 +1384,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" s="15" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="15" t="n">
+    <row r="19" s="10" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="10" t="n">
         <v>16</v>
       </c>
       <c r="I19" s="10" t="s">
@@ -1357,7 +1403,7 @@
       <c r="M19" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" s="15" t="s">
         <v>101</v>
       </c>
       <c r="O19" s="10" t="s">
@@ -1367,16 +1413,77 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N20" s="17" t="s">
+    <row r="20" s="10" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>104</v>
       </c>
+      <c r="J20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" s="10" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H21" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="P21" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="18"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K26" s="19"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K26" s="17"/>
+      <c r="N26" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" s="19" customFormat="true" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N27" s="20" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1401,6 +1508,8 @@
     <hyperlink ref="K17" r:id="rId14" display="Link"/>
     <hyperlink ref="K18" r:id="rId15" display="Link"/>
     <hyperlink ref="K19" r:id="rId16" display="Link"/>
+    <hyperlink ref="K20" r:id="rId17" display="Link"/>
+    <hyperlink ref="K21" r:id="rId18" display="Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added necessary codes, user manual and ppt.
</commit_message>
<xml_diff>
--- a/DOCs/BOM.xlsx
+++ b/DOCs/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="144">
   <si>
     <t xml:space="preserve">TRON Programming Contest 2025</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">BOM REV : 0</t>
   </si>
   <si>
+    <t xml:space="preserve">SHRAVYA : A Cognitive Ear Worn Assistant with on-board AI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sr.no</t>
   </si>
   <si>
@@ -115,7 +118,7 @@
     <t xml:space="preserve">10 mm eccentric-mass motor, draws ~100 mA peak, fits inside earbud shell</t>
   </si>
   <si>
-    <t xml:space="preserve">Logic-Level MOSFET </t>
+    <t xml:space="preserve">##Logic-Level MOSFET </t>
   </si>
   <si>
     <t xml:space="preserve">2N7002</t>
@@ -235,7 +238,7 @@
     <t xml:space="preserve">Protected pouch cell, ~22 h runtime with duty-cycled sensing/inference</t>
   </si>
   <si>
-    <t xml:space="preserve">Li-Po Charger IC </t>
+    <t xml:space="preserve">##Li-Po Charger IC </t>
   </si>
   <si>
     <t xml:space="preserve">MCP73831T-2ACI-OT</t>
@@ -366,7 +369,90 @@
     <t xml:space="preserve">Terminates sudden ESD spikes</t>
   </si>
   <si>
-    <t xml:space="preserve">GROSS : Rs. 8540.38</t>
+    <t xml:space="preserve">Li-Po Charger Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP4056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1A Li-Ion Battery Charging Board Micro USB with Current Protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logic Level Mosfet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRLZ44N 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosfet IC Dip-3 Package
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Based Conductive Epoxy and Curing Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 each</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To fix hardware connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To attach the 30AWG wire with the Dry In Ear EEG Electrodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isopropyl Alcohol and Gloves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 + 2 pairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For cleaning and safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To apply on the Electrodes to remove any grease, oil, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECG Electrodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3M Disposable Electrodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 31.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs. 158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To act as reference electrode for the DRL circuit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To retrieve EEG/ECG signals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROSS : Rs. 11,108.38</t>
   </si>
   <si>
     <t xml:space="preserve">***(The gross total also includes delivery charges, which are directly included in the “Total Cost” column)</t>
@@ -380,7 +466,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +497,15 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Latin Modern Math"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -457,20 +552,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Latin Modern Math"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Latin Modern Math"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -530,11 +623,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -551,71 +644,75 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -869,10 +966,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="F1:R27"/>
+  <dimension ref="F1:R28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N27" activeCellId="0" sqref="N27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -882,7 +979,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="24.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="38.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="85.17"/>
   </cols>
@@ -896,42 +993,46 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="J2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" s="8" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,28 +1041,28 @@
         <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" s="10" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,28 +1070,28 @@
         <v>2</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L5" s="10" t="n">
         <v>3</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" s="8" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,28 +1100,28 @@
         <v>3</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L6" s="10" t="n">
         <v>2</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,28 +1131,28 @@
         <v>4</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L7" s="10" t="n">
         <v>4</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,28 +1162,28 @@
         <v>5</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L8" s="10" t="n">
         <v>2</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" s="8" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,28 +1192,28 @@
         <v>6</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" s="8" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,28 +1222,28 @@
         <v>7</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" s="12" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,28 +1252,28 @@
         <v>8</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L11" s="10" t="n">
         <v>10</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" s="8" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,28 +1282,28 @@
         <v>9</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" s="8" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,28 +1312,28 @@
         <v>10</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L13" s="10" t="n">
         <v>2</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" s="8" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,28 +1342,28 @@
         <v>11</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L14" s="10" t="n">
         <v>2</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P14" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" s="8" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,28 +1372,28 @@
         <v>12</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" s="10" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,28 +1401,28 @@
         <v>13</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L16" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
@@ -1331,28 +1432,28 @@
         <v>14</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L17" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" s="10" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1360,28 +1461,28 @@
         <v>15</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L18" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" s="10" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,28 +1490,28 @@
         <v>16</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L19" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P19" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" s="10" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,28 +1519,28 @@
         <v>17</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L20" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" s="10" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,49 +1548,190 @@
         <v>18</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L21" s="10" t="n">
         <v>10</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="16"/>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K26" s="17"/>
-      <c r="N26" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" s="19" customFormat="true" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" s="11" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" s="11" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" s="10" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="10" t="n">
+        <v>21</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" s="10" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="10" t="n">
+        <v>22</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" s="17" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H26" s="17" t="n">
+        <v>23</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="L26" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="O26" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" s="19" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="N27" s="20" t="s">
-        <v>115</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N28" s="21" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" display="Link"/>
@@ -1510,6 +1752,8 @@
     <hyperlink ref="K19" r:id="rId16" display="Link"/>
     <hyperlink ref="K20" r:id="rId17" display="Link"/>
     <hyperlink ref="K21" r:id="rId18" display="Link"/>
+    <hyperlink ref="K22" r:id="rId19" display="Link"/>
+    <hyperlink ref="K23" r:id="rId20" display="Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>